<commit_message>
intermediate commit to change names
</commit_message>
<xml_diff>
--- a/t/test_files/TestBook.xlsx
+++ b/t/test_files/TestBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="6720" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="15150" windowHeight="4455" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -13,13 +13,13 @@
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Hello</t>
   </si>
@@ -28,6 +28,42 @@
   </si>
   <si>
     <t>my</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Omaha</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Superbowl Audibles</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>2/6/2011</t>
   </si>
   <si>
     <r>
@@ -42,44 +78,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>llo</t>
+      <t xml:space="preserve">llo </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Omaha</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Superbowl Audibles</t>
-  </si>
-  <si>
-    <t>Column Labels</t>
-  </si>
-  <si>
-    <t>2/6/2011</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>World</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -89,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +120,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -146,8 +165,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -228,7 +251,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:E6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -590,18 +613,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -612,7 +635,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -623,7 +646,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -634,7 +657,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -645,7 +668,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>30</v>
@@ -656,7 +679,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -689,15 +712,15 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>40944</v>
@@ -709,12 +732,12 @@
         <v>41672</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>10</v>
@@ -729,7 +752,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -742,7 +765,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>30</v>
@@ -759,7 +782,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>40</v>
@@ -781,10 +804,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -793,7 +816,7 @@
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -801,22 +824,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75">
       <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+    <row r="5" spans="1:6" ht="26.25">
+      <c r="A5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="B6">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="B7">
         <v>27</v>
       </c>
@@ -824,38 +848,50 @@
         <v>37145</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="B8">
         <f>B6-B7</f>
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="D9" s="1"/>
       <c r="E9" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>14</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="8">
         <v>2.1345678901</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="D11" s="9">
+    <row r="11" spans="1:6">
+      <c r="D11" s="10">
         <f>DATEVALUE(E9)</f>
         <v>39118</v>
       </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="E11" s="10"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D13" s="9">
+        <f>D11</f>
+        <v>39118</v>
+      </c>
+      <c r="E13" s="2">
+        <f>D13</f>
+        <v>39118</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="4" r:id="rId1"/>

</xml_diff>

<commit_message>
+ Initial near CPAN Release with a full test suit for cross platform testing + Changed the Cell class to be just an encapulated data holder ! Fixed the resources links in the META files + Used type support from Type::Coercions to allow for data transformation definitions ! The documentation is all wrong.  Next release I promise! ! Reader parsing support only 	- DOM parsing contract dependant or some (possibly distant) time in the future
</commit_message>
<xml_diff>
--- a/t/test_files/TestBook.xlsx
+++ b/t/test_files/TestBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="15150" windowHeight="4455" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="15150" windowHeight="4455" tabRatio="505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:E6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -804,10 +804,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -816,82 +816,82 @@
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
-      <c r="C3" s="7" t="s">
+    <row r="4" spans="1:6" ht="18.75">
+      <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26.25">
-      <c r="A5" s="11" t="s">
+    <row r="6" spans="1:6" ht="26.25">
+      <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="11"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="B6">
-        <v>69</v>
-      </c>
+      <c r="B6" s="11"/>
     </row>
     <row r="7" spans="1:6">
       <c r="B7">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2">
-        <v>37145</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8">
-        <f>B6-B7</f>
+        <v>27</v>
+      </c>
+      <c r="E8" s="2">
+        <v>37145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9">
+        <f>B7-B8</f>
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="D9" s="1"/>
-      <c r="E9" s="6" t="s">
+    <row r="10" spans="1:6">
+      <c r="D10" s="1"/>
+      <c r="E10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="8">
+    <row r="11" spans="1:6">
+      <c r="A11" s="8">
         <v>2.1345678901</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="D11" s="10">
-        <f>DATEVALUE(E9)</f>
+    <row r="12" spans="1:6">
+      <c r="D12" s="10">
+        <f>DATEVALUE(E10)</f>
         <v>39118</v>
       </c>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13" t="s">
+      <c r="E12" s="10"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="9">
-        <f>D11</f>
+      <c r="D14" s="9">
+        <f>D12</f>
         <v>39118</v>
       </c>
-      <c r="E13" s="2">
-        <f>D13</f>
+      <c r="E14" s="2">
+        <f>D14</f>
         <v>39118</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="4" r:id="rId1"/>

</xml_diff>

<commit_message>
! Fixed a bug in the error reporting for the value method in the cell ! Fixed a bug where the sheet position wasn't set correctly when calling for worksheet generation by name 	added a test file for this case ! Improved temp dir cleanup in error situations - with less code 	this inclues a new explicit DEMOLISH at the cell level
</commit_message>
<xml_diff>
--- a/t/test_files/TestBook.xlsx
+++ b/t/test_files/TestBook.xlsx
@@ -698,7 +698,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -807,7 +807,7 @@
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -859,7 +859,7 @@
       <c r="E10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
! Closed #40 in github thanks @wdbaker54
</commit_message>
<xml_diff>
--- a/t/test_files/TestBook.xlsx
+++ b/t/test_files/TestBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="9345" windowHeight="4455" tabRatio="505" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="9345" windowHeight="4455" tabRatio="505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Hello</t>
   </si>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -690,6 +690,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -806,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -855,7 +856,9 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E10" s="6" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
! Closed #42 in github
</commit_message>
<xml_diff>
--- a/t/test_files/TestBook.xlsx
+++ b/t/test_files/TestBook.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:E6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -603,7 +603,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -618,7 +618,7 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>